<commit_message>
fully bo, mle-bo calibrations add
</commit_message>
<xml_diff>
--- a/data/Bolometer_readings_under_the_cone_new_old.xlsx
+++ b/data/Bolometer_readings_under_the_cone_new_old.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valenetjong/Bayesian-Optimization-Ferroelectrics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5371370-4435-7144-A664-F513B872C7BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51209FF4-FD0E-E349-9725-AE5D1BC53F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="56960" yWindow="500" windowWidth="23040" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="56960" yWindow="500" windowWidth="23040" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calibrations" sheetId="1" r:id="rId1"/>
@@ -491,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:I44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1661,7 +1661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A63D0C59-5EC6-AA44-B57C-2A690131BC74}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -2790,7 +2790,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{504722A9-62E2-405D-AB2A-3E1490BC7F79}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>